<commit_message>
fixed feature selection logic
</commit_message>
<xml_diff>
--- a/Export/FeatureSelection_LawSuit.xlsx
+++ b/Export/FeatureSelection_LawSuit.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cdc4f9836624c718/Documents/Grad-School-Docs/CapstoneProject/Repo/Export/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_FFC65FC03C69AAD9F8526FDDB5A860DF61B4EB33" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5371799-795D-4DDA-B66A-BDF537B984B6}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="50">
   <si>
     <t>feature</t>
   </si>
@@ -31,115 +25,133 @@
     <t>Model</t>
   </si>
   <si>
+    <t>caps</t>
+  </si>
+  <si>
+    <t>sstk_std</t>
+  </si>
+  <si>
+    <t>sstk</t>
+  </si>
+  <si>
+    <t>teq</t>
+  </si>
+  <si>
+    <t>ceqt</t>
+  </si>
+  <si>
     <t>rest_sum_diff</t>
   </si>
   <si>
-    <t>st_prc_end</t>
-  </si>
-  <si>
-    <t>teq</t>
-  </si>
-  <si>
-    <t>caps</t>
-  </si>
-  <si>
-    <t>cibegni_std</t>
-  </si>
-  <si>
-    <t>sstk_std</t>
-  </si>
-  <si>
-    <t>epsfi_std</t>
+    <t>ceq</t>
+  </si>
+  <si>
+    <t>at</t>
+  </si>
+  <si>
+    <t>xsga_std</t>
+  </si>
+  <si>
+    <t>st_per_growth</t>
+  </si>
+  <si>
+    <t>rest_count</t>
   </si>
   <si>
     <t>seq</t>
   </si>
   <si>
-    <t>bkvlps</t>
-  </si>
-  <si>
-    <t>ceq</t>
+    <t>pi_std</t>
+  </si>
+  <si>
+    <t>xacc</t>
+  </si>
+  <si>
+    <t>xsga</t>
+  </si>
+  <si>
+    <t>intpn</t>
+  </si>
+  <si>
+    <t>cogs_std</t>
+  </si>
+  <si>
+    <t>xopr</t>
+  </si>
+  <si>
+    <t>cogs</t>
+  </si>
+  <si>
+    <t>wcap</t>
+  </si>
+  <si>
+    <t>fopo_std</t>
+  </si>
+  <si>
+    <t>gp_std</t>
   </si>
   <si>
     <t>gp</t>
   </si>
   <si>
-    <t>ceqt</t>
-  </si>
-  <si>
-    <t>ppegt</t>
+    <t>icapt</t>
+  </si>
+  <si>
+    <t>dp</t>
+  </si>
+  <si>
+    <t>sec_trt1m_std</t>
+  </si>
+  <si>
+    <t>revt</t>
+  </si>
+  <si>
+    <t>dlc</t>
+  </si>
+  <si>
+    <t>tstk_std</t>
+  </si>
+  <si>
+    <t>lse_std</t>
+  </si>
+  <si>
+    <t>dilavx_std</t>
+  </si>
+  <si>
+    <t>ch</t>
+  </si>
+  <si>
+    <t>lse</t>
   </si>
   <si>
     <t>rest_count_of_diffs</t>
   </si>
   <si>
-    <t>esubc</t>
-  </si>
-  <si>
-    <t>lct</t>
-  </si>
-  <si>
-    <t>tstk</t>
-  </si>
-  <si>
-    <t>sec_trt1m_std</t>
-  </si>
-  <si>
-    <t>cshpri_std</t>
-  </si>
-  <si>
-    <t>cogs_std</t>
-  </si>
-  <si>
-    <t>epspi_std</t>
-  </si>
-  <si>
-    <t>lse</t>
-  </si>
-  <si>
-    <t>oancf</t>
-  </si>
-  <si>
-    <t>at</t>
-  </si>
-  <si>
-    <t>caps_std</t>
+    <t>aoloch</t>
   </si>
   <si>
     <t>auop</t>
   </si>
   <si>
-    <t>ni_std</t>
-  </si>
-  <si>
-    <t>dilavx_std</t>
-  </si>
-  <si>
-    <t>dlc</t>
-  </si>
-  <si>
-    <t>ci</t>
-  </si>
-  <si>
-    <t>nopi_std</t>
-  </si>
-  <si>
-    <t>opeps_std</t>
+    <t>dvc_std</t>
+  </si>
+  <si>
+    <t>sec_trt1m_mean</t>
+  </si>
+  <si>
+    <t>lct_std</t>
   </si>
   <si>
     <t>fincf</t>
   </si>
   <si>
-    <t>prca</t>
-  </si>
-  <si>
-    <t>fincf_std</t>
-  </si>
-  <si>
-    <t>sec_ajpm</t>
-  </si>
-  <si>
-    <t>sec_trfm_mean</t>
+    <t>spce_std</t>
+  </si>
+  <si>
+    <t>st_volatility</t>
+  </si>
+  <si>
+    <t>dltr</t>
   </si>
   <si>
     <t>rat_spcsrc</t>
@@ -157,8 +169,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -221,14 +233,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -275,7 +279,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -307,27 +311,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -359,24 +345,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -552,21 +520,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D48"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -577,7 +538,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -585,13 +546,13 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>3.180438687351881E-2</v>
+        <v>0.05236128050729389</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -599,13 +560,13 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>3.0451400546941901E-2</v>
+        <v>0.04444672378099979</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -613,13 +574,13 @@
         <v>5</v>
       </c>
       <c r="C4">
-        <v>2.8339118379799331E-2</v>
+        <v>0.0260241879881601</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -627,13 +588,13 @@
         <v>6</v>
       </c>
       <c r="C5">
-        <v>2.540864978579346E-2</v>
+        <v>0.02540094764238473</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -641,13 +602,13 @@
         <v>7</v>
       </c>
       <c r="C6">
-        <v>2.5231439619679139E-2</v>
+        <v>0.02146115414763942</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -655,13 +616,13 @@
         <v>8</v>
       </c>
       <c r="C7">
-        <v>2.0214390523775109E-2</v>
+        <v>0.02121926403098512</v>
       </c>
       <c r="D7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -669,13 +630,13 @@
         <v>9</v>
       </c>
       <c r="C8">
-        <v>1.9867256879183538E-2</v>
+        <v>0.0194860830485395</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -683,13 +644,13 @@
         <v>10</v>
       </c>
       <c r="C9">
-        <v>1.901275889866345E-2</v>
+        <v>0.01894903653076352</v>
       </c>
       <c r="D9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -697,13 +658,13 @@
         <v>11</v>
       </c>
       <c r="C10">
-        <v>1.7304983364270912E-2</v>
+        <v>0.01859904176761554</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -711,13 +672,13 @@
         <v>12</v>
       </c>
       <c r="C11">
-        <v>1.657170922924019E-2</v>
+        <v>0.01848543000309096</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -725,13 +686,13 @@
         <v>13</v>
       </c>
       <c r="C12">
-        <v>1.585183062586018E-2</v>
+        <v>0.01751978001997758</v>
       </c>
       <c r="D12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -739,13 +700,13 @@
         <v>14</v>
       </c>
       <c r="C13">
-        <v>1.465199479859576E-2</v>
+        <v>0.01741619803266959</v>
       </c>
       <c r="D13" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -753,13 +714,13 @@
         <v>15</v>
       </c>
       <c r="C14">
-        <v>1.294480709949819E-2</v>
+        <v>0.01717798853639354</v>
       </c>
       <c r="D14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -767,13 +728,13 @@
         <v>16</v>
       </c>
       <c r="C15">
-        <v>1.2717270067856791E-2</v>
+        <v>0.01675076321598326</v>
       </c>
       <c r="D15" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -781,13 +742,13 @@
         <v>17</v>
       </c>
       <c r="C16">
-        <v>1.246960674468268E-2</v>
+        <v>0.01671246205823291</v>
       </c>
       <c r="D16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -795,13 +756,13 @@
         <v>18</v>
       </c>
       <c r="C17">
-        <v>1.224527733108407E-2</v>
+        <v>0.01601259109436687</v>
       </c>
       <c r="D17" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -809,13 +770,13 @@
         <v>19</v>
       </c>
       <c r="C18">
-        <v>1.127047263800693E-2</v>
+        <v>0.015629214618714</v>
       </c>
       <c r="D18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -823,13 +784,13 @@
         <v>20</v>
       </c>
       <c r="C19">
-        <v>1.1173032158961959E-2</v>
+        <v>0.01532219756584577</v>
       </c>
       <c r="D19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -837,13 +798,13 @@
         <v>21</v>
       </c>
       <c r="C20">
-        <v>1.103369051894184E-2</v>
+        <v>0.01493664561795656</v>
       </c>
       <c r="D20" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -851,13 +812,13 @@
         <v>22</v>
       </c>
       <c r="C21">
-        <v>1.0937415477209771E-2</v>
+        <v>0.01461114291310617</v>
       </c>
       <c r="D21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -865,13 +826,13 @@
         <v>23</v>
       </c>
       <c r="C22">
-        <v>1.093446409819436E-2</v>
+        <v>0.01370301894502899</v>
       </c>
       <c r="D22" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -879,13 +840,13 @@
         <v>24</v>
       </c>
       <c r="C23">
-        <v>1.0608901717781789E-2</v>
+        <v>0.01330009415677367</v>
       </c>
       <c r="D23" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -893,13 +854,13 @@
         <v>25</v>
       </c>
       <c r="C24">
-        <v>1.0479125311664551E-2</v>
+        <v>0.0132734509903946</v>
       </c>
       <c r="D24" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -907,332 +868,570 @@
         <v>26</v>
       </c>
       <c r="C25">
-        <v>0.18675649935554031</v>
+        <v>0.01271241124677915</v>
       </c>
       <c r="D25" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="C26">
-        <v>0.1042154006180281</v>
+        <v>0.01250753168455382</v>
       </c>
       <c r="D26" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" s="1">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="C27">
-        <v>6.0853785931871837E-2</v>
+        <v>0.01204080358569956</v>
       </c>
       <c r="D27" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C28">
-        <v>5.9463010744599788E-2</v>
+        <v>0.01183693316225474</v>
       </c>
       <c r="D28" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C29">
-        <v>3.6678722040558609E-2</v>
+        <v>0.0114149739805837</v>
       </c>
       <c r="D29" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" s="1">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="C30">
-        <v>2.8577647925420911E-2</v>
+        <v>0.01131284344408935</v>
       </c>
       <c r="D30" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" s="1">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C31">
-        <v>2.8162644825896251E-2</v>
+        <v>0.01113117619351423</v>
       </c>
       <c r="D31" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" s="1">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C32">
-        <v>2.423804210594506E-2</v>
+        <v>0.01110369304488112</v>
       </c>
       <c r="D32" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" s="1">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C33">
-        <v>2.3287815281033832E-2</v>
+        <v>0.01076532666388239</v>
       </c>
       <c r="D33" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C34">
-        <v>2.2087540118266091E-2</v>
+        <v>0.01061612778108777</v>
       </c>
       <c r="D34" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" s="1">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="C35">
-        <v>2.177827016036047E-2</v>
+        <v>0.01056611143324408</v>
       </c>
       <c r="D35" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C36">
-        <v>1.7213169353714221E-2</v>
+        <v>0.01056012943955755</v>
       </c>
       <c r="D36" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" s="1">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="C37">
-        <v>1.654539880936207E-2</v>
+        <v>0.01020394994577533</v>
       </c>
       <c r="D37" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" s="1">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C38">
-        <v>1.506166404548028E-2</v>
+        <v>0.1656787033117564</v>
       </c>
       <c r="D38" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" s="1">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C39">
-        <v>1.4987850848130471E-2</v>
+        <v>0.05543152335079476</v>
       </c>
       <c r="D39" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40" s="1">
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C40">
-        <v>1.4554938826128081E-2</v>
+        <v>0.05522235382194401</v>
       </c>
       <c r="D40" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41" s="1">
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C41">
-        <v>1.385516018435399E-2</v>
+        <v>0.04998705038417583</v>
       </c>
       <c r="D41" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42" s="1">
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="C42">
-        <v>1.257025173637938E-2</v>
+        <v>0.04819093790619966</v>
       </c>
       <c r="D42" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43" s="1">
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C43">
-        <v>1.1939828914875409E-2</v>
+        <v>0.04646944956788315</v>
       </c>
       <c r="D43" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" s="1">
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="C44">
-        <v>1.149704012772629E-2</v>
+        <v>0.03583009220339297</v>
       </c>
       <c r="D44" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45" s="1">
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="C45">
-        <v>1.1140493502494769E-2</v>
+        <v>0.03288531214389128</v>
       </c>
       <c r="D45" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46" s="1">
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="C46">
-        <v>1.068436476339635E-2</v>
+        <v>0.03194837004505835</v>
       </c>
       <c r="D46" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47" s="1">
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="C47">
-        <v>1.0318176837072901E-2</v>
+        <v>0.03014599349210568</v>
       </c>
       <c r="D47" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48" s="1">
         <v>46</v>
       </c>
       <c r="B48" t="s">
+        <v>19</v>
+      </c>
+      <c r="C48">
+        <v>0.0280241868029258</v>
+      </c>
+      <c r="D48" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="1">
+        <v>47</v>
+      </c>
+      <c r="B49" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49">
+        <v>0.02320045073336028</v>
+      </c>
+      <c r="D49" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="1">
+        <v>48</v>
+      </c>
+      <c r="B50" t="s">
         <v>40</v>
       </c>
-      <c r="C48">
-        <v>1.111E-3</v>
-      </c>
-      <c r="D48" t="s">
+      <c r="C50">
+        <v>0.023055316966426</v>
+      </c>
+      <c r="D50" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="1">
+        <v>49</v>
+      </c>
+      <c r="B51" t="s">
+        <v>41</v>
+      </c>
+      <c r="C51">
+        <v>0.02102212378493936</v>
+      </c>
+      <c r="D51" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="1">
+        <v>50</v>
+      </c>
+      <c r="B52" t="s">
+        <v>13</v>
+      </c>
+      <c r="C52">
+        <v>0.02095247136336931</v>
+      </c>
+      <c r="D52" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="1">
+        <v>51</v>
+      </c>
+      <c r="B53" t="s">
+        <v>27</v>
+      </c>
+      <c r="C53">
+        <v>0.02088377035741677</v>
+      </c>
+      <c r="D53" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="1">
+        <v>52</v>
+      </c>
+      <c r="B54" t="s">
+        <v>12</v>
+      </c>
+      <c r="C54">
+        <v>0.01881978604738369</v>
+      </c>
+      <c r="D54" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="1">
+        <v>53</v>
+      </c>
+      <c r="B55" t="s">
+        <v>22</v>
+      </c>
+      <c r="C55">
+        <v>0.01731557477188951</v>
+      </c>
+      <c r="D55" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="1">
+        <v>54</v>
+      </c>
+      <c r="B56" t="s">
+        <v>42</v>
+      </c>
+      <c r="C56">
+        <v>0.01600023941382228</v>
+      </c>
+      <c r="D56" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="1">
+        <v>55</v>
+      </c>
+      <c r="B57" t="s">
+        <v>35</v>
+      </c>
+      <c r="C57">
+        <v>0.01506718967266691</v>
+      </c>
+      <c r="D57" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="1">
+        <v>56</v>
+      </c>
+      <c r="B58" t="s">
+        <v>30</v>
+      </c>
+      <c r="C58">
+        <v>0.01438069669873015</v>
+      </c>
+      <c r="D58" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="1">
+        <v>57</v>
+      </c>
+      <c r="B59" t="s">
+        <v>3</v>
+      </c>
+      <c r="C59">
+        <v>0.01392014980785209</v>
+      </c>
+      <c r="D59" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="1">
+        <v>58</v>
+      </c>
+      <c r="B60" t="s">
+        <v>37</v>
+      </c>
+      <c r="C60">
+        <v>0.01336995819009633</v>
+      </c>
+      <c r="D60" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="1">
+        <v>59</v>
+      </c>
+      <c r="B61" t="s">
+        <v>9</v>
+      </c>
+      <c r="C61">
+        <v>0.0120456807073082</v>
+      </c>
+      <c r="D61" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="1">
+        <v>60</v>
+      </c>
+      <c r="B62" t="s">
         <v>43</v>
+      </c>
+      <c r="C62">
+        <v>0.01178048360405561</v>
+      </c>
+      <c r="D62" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="1">
+        <v>61</v>
+      </c>
+      <c r="B63" t="s">
+        <v>44</v>
+      </c>
+      <c r="C63">
+        <v>0.0117718601034206</v>
+      </c>
+      <c r="D63" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="1">
+        <v>62</v>
+      </c>
+      <c r="B64" t="s">
+        <v>45</v>
+      </c>
+      <c r="C64">
+        <v>0.0105075454579322</v>
+      </c>
+      <c r="D64" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="1">
+        <v>63</v>
+      </c>
+      <c r="B65" t="s">
+        <v>46</v>
+      </c>
+      <c r="C65">
+        <v>0.001111</v>
+      </c>
+      <c r="D65" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
alt feature selection configured
</commit_message>
<xml_diff>
--- a/Export/FeatureSelection_LawSuit.xlsx
+++ b/Export/FeatureSelection_LawSuit.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="53">
   <si>
     <t>feature</t>
   </si>
@@ -25,136 +25,142 @@
     <t>Model</t>
   </si>
   <si>
+    <t>xopr</t>
+  </si>
+  <si>
+    <t>caps</t>
+  </si>
+  <si>
+    <t>seq</t>
+  </si>
+  <si>
+    <t>ceq</t>
+  </si>
+  <si>
+    <t>pi_std</t>
+  </si>
+  <si>
     <t>sstk_std</t>
   </si>
   <si>
-    <t>caps</t>
-  </si>
-  <si>
-    <t>seq</t>
+    <t>cogs_std</t>
+  </si>
+  <si>
+    <t>dp</t>
   </si>
   <si>
     <t>rest_sum_diff</t>
   </si>
   <si>
+    <t>sstk</t>
+  </si>
+  <si>
+    <t>xopr_std</t>
+  </si>
+  <si>
+    <t>lse</t>
+  </si>
+  <si>
+    <t>teq</t>
+  </si>
+  <si>
+    <t>rest_a_count_of_diffs</t>
+  </si>
+  <si>
+    <t>gp</t>
+  </si>
+  <si>
+    <t>at_std</t>
+  </si>
+  <si>
+    <t>icapt</t>
+  </si>
+  <si>
+    <t>rest_count_of_diffs</t>
+  </si>
+  <si>
+    <t>revt</t>
+  </si>
+  <si>
+    <t>fopo_std</t>
+  </si>
+  <si>
+    <t>xsga</t>
+  </si>
+  <si>
+    <t>at</t>
+  </si>
+  <si>
+    <t>tstk</t>
+  </si>
+  <si>
+    <t>ceqt</t>
+  </si>
+  <si>
+    <t>rest_count</t>
+  </si>
+  <si>
+    <t>dilavx_std</t>
+  </si>
+  <si>
+    <t>lct</t>
+  </si>
+  <si>
+    <t>ceq_std</t>
+  </si>
+  <si>
+    <t>seq_std</t>
+  </si>
+  <si>
+    <t>invt</t>
+  </si>
+  <si>
     <t>sec_trt1m_std</t>
   </si>
   <si>
-    <t>pi_std</t>
-  </si>
-  <si>
-    <t>ceq</t>
-  </si>
-  <si>
-    <t>xopr</t>
-  </si>
-  <si>
-    <t>ceqt</t>
-  </si>
-  <si>
-    <t>revt</t>
-  </si>
-  <si>
-    <t>cogs_std</t>
-  </si>
-  <si>
-    <t>fopo_std</t>
-  </si>
-  <si>
-    <t>sstk</t>
-  </si>
-  <si>
-    <t>tstk</t>
-  </si>
-  <si>
-    <t>st_per_growth</t>
-  </si>
-  <si>
-    <t>teq</t>
-  </si>
-  <si>
-    <t>icapt</t>
-  </si>
-  <si>
-    <t>lse</t>
-  </si>
-  <si>
-    <t>xopr_std</t>
-  </si>
-  <si>
-    <t>rest_count</t>
-  </si>
-  <si>
-    <t>rest_count_of_diffs</t>
-  </si>
-  <si>
-    <t>at</t>
-  </si>
-  <si>
-    <t>dp</t>
-  </si>
-  <si>
-    <t>lct</t>
-  </si>
-  <si>
-    <t>xsga</t>
-  </si>
-  <si>
-    <t>gp</t>
-  </si>
-  <si>
-    <t>cogs</t>
-  </si>
-  <si>
-    <t>dilavx_std</t>
-  </si>
-  <si>
-    <t>rest_a_count_of_diffs</t>
+    <t>tot_tax_std</t>
+  </si>
+  <si>
+    <t>icapt_std</t>
+  </si>
+  <si>
+    <t>xsga_std</t>
   </si>
   <si>
     <t>xacc_std</t>
   </si>
   <si>
+    <t>wcap</t>
+  </si>
+  <si>
+    <t>ppegt</t>
+  </si>
+  <si>
+    <t>aoloch</t>
+  </si>
+  <si>
     <t>dlc</t>
   </si>
   <si>
     <t>intpn</t>
   </si>
   <si>
-    <t>at_std</t>
-  </si>
-  <si>
-    <t>dvc_std</t>
-  </si>
-  <si>
-    <t>xsga_std</t>
-  </si>
-  <si>
-    <t>ivncf</t>
-  </si>
-  <si>
-    <t>ppegt</t>
-  </si>
-  <si>
-    <t>cshpri</t>
-  </si>
-  <si>
-    <t>spce</t>
-  </si>
-  <si>
-    <t>np_std</t>
-  </si>
-  <si>
-    <t>wcap</t>
-  </si>
-  <si>
-    <t>gvkey</t>
-  </si>
-  <si>
-    <t>st_per_currentToMax</t>
-  </si>
-  <si>
-    <t>spce_std</t>
+    <t>ebit</t>
+  </si>
+  <si>
+    <t>lct_std</t>
+  </si>
+  <si>
+    <t>pi</t>
+  </si>
+  <si>
+    <t>invt_std</t>
+  </si>
+  <si>
+    <t>teq_std</t>
+  </si>
+  <si>
+    <t>re</t>
   </si>
   <si>
     <t>rat_spcsrc</t>
@@ -524,7 +530,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:D58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -549,10 +555,10 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>0.0493764537278055</v>
+        <v>0.05936836012536634</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -563,10 +569,10 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>0.03181429044536385</v>
+        <v>0.04448085585593663</v>
       </c>
       <c r="D3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -577,10 +583,10 @@
         <v>5</v>
       </c>
       <c r="C4">
-        <v>0.02953661657792137</v>
+        <v>0.04330364829327429</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -591,10 +597,10 @@
         <v>6</v>
       </c>
       <c r="C5">
-        <v>0.02626963088369082</v>
+        <v>0.04155522263896471</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -605,10 +611,10 @@
         <v>7</v>
       </c>
       <c r="C6">
-        <v>0.02494683602758725</v>
+        <v>0.04031362597108206</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -619,10 +625,10 @@
         <v>8</v>
       </c>
       <c r="C7">
-        <v>0.02447587271462206</v>
+        <v>0.03908932476392177</v>
       </c>
       <c r="D7" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -633,10 +639,10 @@
         <v>9</v>
       </c>
       <c r="C8">
-        <v>0.02326934168269541</v>
+        <v>0.03843676832212337</v>
       </c>
       <c r="D8" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -647,10 +653,10 @@
         <v>10</v>
       </c>
       <c r="C9">
-        <v>0.02195226062919785</v>
+        <v>0.0379425788551238</v>
       </c>
       <c r="D9" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -661,10 +667,10 @@
         <v>11</v>
       </c>
       <c r="C10">
-        <v>0.02144030186801744</v>
+        <v>0.03595357638258925</v>
       </c>
       <c r="D10" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -675,10 +681,10 @@
         <v>12</v>
       </c>
       <c r="C11">
-        <v>0.02078931939598285</v>
+        <v>0.03238683576569578</v>
       </c>
       <c r="D11" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -689,10 +695,10 @@
         <v>13</v>
       </c>
       <c r="C12">
-        <v>0.02073931992611006</v>
+        <v>0.03088900684995909</v>
       </c>
       <c r="D12" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -703,10 +709,10 @@
         <v>14</v>
       </c>
       <c r="C13">
-        <v>0.01910649965211146</v>
+        <v>0.0253438264160008</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -717,10 +723,10 @@
         <v>15</v>
       </c>
       <c r="C14">
-        <v>0.01896011813660929</v>
+        <v>0.02491401808079273</v>
       </c>
       <c r="D14" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -731,10 +737,10 @@
         <v>16</v>
       </c>
       <c r="C15">
-        <v>0.01681057022309305</v>
+        <v>0.02392882786457341</v>
       </c>
       <c r="D15" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -745,10 +751,10 @@
         <v>17</v>
       </c>
       <c r="C16">
-        <v>0.0162058398940578</v>
+        <v>0.0233902266769408</v>
       </c>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -759,10 +765,10 @@
         <v>18</v>
       </c>
       <c r="C17">
-        <v>0.01589937568216011</v>
+        <v>0.02287440902780302</v>
       </c>
       <c r="D17" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -773,10 +779,10 @@
         <v>19</v>
       </c>
       <c r="C18">
-        <v>0.01578149754426245</v>
+        <v>0.02203483965053024</v>
       </c>
       <c r="D18" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -787,10 +793,10 @@
         <v>20</v>
       </c>
       <c r="C19">
-        <v>0.01527458192311974</v>
+        <v>0.02081628755925887</v>
       </c>
       <c r="D19" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -801,10 +807,10 @@
         <v>21</v>
       </c>
       <c r="C20">
-        <v>0.01499243398764296</v>
+        <v>0.02034944590047191</v>
       </c>
       <c r="D20" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -815,10 +821,10 @@
         <v>22</v>
       </c>
       <c r="C21">
-        <v>0.01457794342027231</v>
+        <v>0.01876608405328162</v>
       </c>
       <c r="D21" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -829,10 +835,10 @@
         <v>23</v>
       </c>
       <c r="C22">
-        <v>0.01414685508385125</v>
+        <v>0.01640542831968089</v>
       </c>
       <c r="D22" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -843,10 +849,10 @@
         <v>24</v>
       </c>
       <c r="C23">
-        <v>0.01403566806788875</v>
+        <v>0.0153984767811917</v>
       </c>
       <c r="D23" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -857,10 +863,10 @@
         <v>25</v>
       </c>
       <c r="C24">
-        <v>0.01324615809200946</v>
+        <v>0.01512782779687607</v>
       </c>
       <c r="D24" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -871,10 +877,10 @@
         <v>26</v>
       </c>
       <c r="C25">
-        <v>0.01316860895018597</v>
+        <v>0.01417570923072858</v>
       </c>
       <c r="D25" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -885,10 +891,10 @@
         <v>27</v>
       </c>
       <c r="C26">
-        <v>0.01229883760396171</v>
+        <v>0.01370577589896684</v>
       </c>
       <c r="D26" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -899,10 +905,10 @@
         <v>28</v>
       </c>
       <c r="C27">
-        <v>0.01223397244347807</v>
+        <v>0.01356600908861781</v>
       </c>
       <c r="D27" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -913,10 +919,10 @@
         <v>29</v>
       </c>
       <c r="C28">
-        <v>0.01181015337884055</v>
+        <v>0.01340536308183276</v>
       </c>
       <c r="D28" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -927,10 +933,10 @@
         <v>30</v>
       </c>
       <c r="C29">
-        <v>0.01146970697463186</v>
+        <v>0.01318991684277836</v>
       </c>
       <c r="D29" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -941,10 +947,10 @@
         <v>31</v>
       </c>
       <c r="C30">
-        <v>0.01146720115041226</v>
+        <v>0.0125181251162253</v>
       </c>
       <c r="D30" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -955,10 +961,10 @@
         <v>32</v>
       </c>
       <c r="C31">
-        <v>0.0113170292223706</v>
+        <v>0.01203810800814309</v>
       </c>
       <c r="D31" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -969,10 +975,10 @@
         <v>33</v>
       </c>
       <c r="C32">
-        <v>0.01109259860372374</v>
+        <v>0.0118863223393106</v>
       </c>
       <c r="D32" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -983,10 +989,10 @@
         <v>34</v>
       </c>
       <c r="C33">
-        <v>0.01025947816114036</v>
+        <v>0.01152243565755262</v>
       </c>
       <c r="D33" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -997,10 +1003,10 @@
         <v>35</v>
       </c>
       <c r="C34">
-        <v>0.01008281972998364</v>
+        <v>0.01112284749121236</v>
       </c>
       <c r="D34" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1008,13 +1014,13 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C35">
-        <v>0.1818568884296849</v>
+        <v>0.2489896555961564</v>
       </c>
       <c r="D35" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1022,13 +1028,13 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="C36">
-        <v>0.07243449831639052</v>
+        <v>0.08476524991430098</v>
       </c>
       <c r="D36" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1036,13 +1042,13 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="C37">
-        <v>0.07083684701294128</v>
+        <v>0.05767873440493259</v>
       </c>
       <c r="D37" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1050,13 +1056,13 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="C38">
-        <v>0.06921765598211725</v>
+        <v>0.04496175166378066</v>
       </c>
       <c r="D38" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1064,13 +1070,13 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="C39">
-        <v>0.05795659701669176</v>
+        <v>0.04457452960161186</v>
       </c>
       <c r="D39" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1078,13 +1084,13 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C40">
-        <v>0.03690806782664833</v>
+        <v>0.03102307902394075</v>
       </c>
       <c r="D40" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1092,13 +1098,13 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="C41">
-        <v>0.0324368228024041</v>
+        <v>0.03062149115633627</v>
       </c>
       <c r="D41" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1106,13 +1112,13 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C42">
-        <v>0.03094625821044806</v>
+        <v>0.02980817589259072</v>
       </c>
       <c r="D42" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1120,13 +1126,13 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C43">
-        <v>0.0266783251791956</v>
+        <v>0.02414491915119098</v>
       </c>
       <c r="D43" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1134,13 +1140,13 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C44">
-        <v>0.02559621561844862</v>
+        <v>0.02289107638151175</v>
       </c>
       <c r="D44" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1148,13 +1154,13 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C45">
-        <v>0.02438326073446596</v>
+        <v>0.02158750601264732</v>
       </c>
       <c r="D45" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1162,13 +1168,13 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="C46">
-        <v>0.02433681860013285</v>
+        <v>0.0204572682330454</v>
       </c>
       <c r="D46" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1176,13 +1182,13 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="C47">
-        <v>0.02352321196183267</v>
+        <v>0.01815829815248559</v>
       </c>
       <c r="D47" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1190,13 +1196,13 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C48">
-        <v>0.02239754811756958</v>
+        <v>0.01813984893286448</v>
       </c>
       <c r="D48" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1204,13 +1210,13 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="C49">
-        <v>0.02094690327885315</v>
+        <v>0.01804950712726944</v>
       </c>
       <c r="D49" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1221,10 +1227,10 @@
         <v>43</v>
       </c>
       <c r="C50">
-        <v>0.0152903523540667</v>
+        <v>0.0166728864170848</v>
       </c>
       <c r="D50" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1232,13 +1238,13 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="C51">
-        <v>0.01419499557190307</v>
+        <v>0.01513574990217075</v>
       </c>
       <c r="D51" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1246,13 +1252,13 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="C52">
-        <v>0.01302650405566107</v>
+        <v>0.01385734750181826</v>
       </c>
       <c r="D52" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1260,13 +1266,13 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="C53">
-        <v>0.01174732300039266</v>
+        <v>0.01379666222162135</v>
       </c>
       <c r="D53" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1274,13 +1280,13 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="C54">
-        <v>0.01128016636674957</v>
+        <v>0.01342270523402798</v>
       </c>
       <c r="D54" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1288,13 +1294,13 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="C55">
-        <v>0.01069844239970455</v>
+        <v>0.01171950404716122</v>
       </c>
       <c r="D55" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1302,13 +1308,13 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C56">
-        <v>0.01065452998809641</v>
+        <v>0.01112245010641218</v>
       </c>
       <c r="D56" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1316,13 +1322,13 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C57">
-        <v>0.01057981658342106</v>
+        <v>0.01064486706677645</v>
       </c>
       <c r="D57" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1330,27 +1336,13 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C58">
-        <v>0.01053664008522015</v>
+        <v>0.001111</v>
       </c>
       <c r="D58" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59" s="1">
-        <v>57</v>
-      </c>
-      <c r="B59" t="s">
-        <v>47</v>
-      </c>
-      <c r="C59">
-        <v>0.001111</v>
-      </c>
-      <c r="D59" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>